<commit_message>
upload table sql log aktivitas
</commit_message>
<xml_diff>
--- a/assets/upload/Upload_HAV.xlsx
+++ b/assets/upload/Upload_HAV.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murry Febriansyah P\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\master_ho\assets\upload\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -496,7 +496,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD1048576"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>